<commit_message>
24.10.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/October/Others/Draft Sales target -Rajshahi-October,2020.xlsx
+++ b/2020/October/Others/Draft Sales target -Rajshahi-October,2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7455" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="Distributor Primary" sheetId="1" r:id="rId1"/>
@@ -2097,7 +2097,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2108,13 +2108,13 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:AK21"/>
+  <dimension ref="A1:AK24"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4472,6 +4472,9 @@
         <f t="shared" si="2"/>
         <v>599</v>
       </c>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="AK24" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:AJ21">
@@ -26022,7 +26025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>